<commit_message>
excel upload and osm feature
</commit_message>
<xml_diff>
--- a/frontend/src/assets/excel_examples/TeilnehmerImport BuSiFe2.xlsx
+++ b/frontend/src/assets/excel_examples/TeilnehmerImport BuSiFe2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Documents/privat/Pfadfinder/anmelde-tool/frontend/src/assets/excel_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0721BC4-9A00-FA48-9E91-C4B2E3E9065B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F059E8-FC2D-4A43-9963-420D27D4B1EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20060" xr2:uid="{3E166413-D23F-144E-8F0D-A6F25A4F69F0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Robert</t>
   </si>
@@ -115,6 +115,24 @@
   </si>
   <si>
     <t>Sippestufe</t>
+  </si>
+  <si>
+    <t>Stadt*</t>
+  </si>
+  <si>
+    <t>40882</t>
+  </si>
+  <si>
+    <t>Ratingen</t>
+  </si>
+  <si>
+    <t>Düsseldorf</t>
+  </si>
+  <si>
+    <t>53113</t>
+  </si>
+  <si>
+    <t>Bonn</t>
   </si>
 </sst>
 </file>
@@ -489,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD2FB9EB-6B35-8149-ABEC-BFAD9299F0C2}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -501,13 +519,13 @@
     <col min="3" max="3" width="15.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" customWidth="1"/>
     <col min="5" max="5" width="13" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17" style="3" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="6" max="7" width="15.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17" style="3" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -527,19 +545,22 @@
         <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -552,20 +573,23 @@
       <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3">
-        <v>12345</v>
+      <c r="F2" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="4">
         <v>40179</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -581,23 +605,26 @@
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="3">
-        <v>11111</v>
+      <c r="F3" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>36735</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -610,24 +637,27 @@
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="3">
-        <v>22222</v>
+      <c r="F4" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>32505</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{E6643557-5ADA-494D-B1A2-4EBB42C55DD0}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{60701480-F839-3743-8576-2AB05918AB54}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{88C9843A-41B2-4A4D-B3D6-34E891B1A4AF}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{E6643557-5ADA-494D-B1A2-4EBB42C55DD0}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{60701480-F839-3743-8576-2AB05918AB54}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{88C9843A-41B2-4A4D-B3D6-34E891B1A4AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>